<commit_message>
feat: create project and multiple modules
- Developed project module to manage project details and associated operations.
- Added Fabric Quantity module to handle fabric quantity requirements for projects.
- Implemented Fabric Price module to manage pricing details for different fabrics.
- Created Logo Printing module for managing logo designs, positions, and pricing logic.
- Built Cutting module to handle cutting operations and costs based on project requirements.
- Developed Stitching module for managing stitching processes and related costs.
- Integrated Packing module to manage the final packing of products.
- Established relationships between modules and project entities for seamless interaction.
- Implemented services, DTOs, and controllers for efficient handling of each module's data.
</commit_message>
<xml_diff>
--- a/data/Shirts/Fabric Pricing.xlsx
+++ b/data/Shirts/Fabric Pricing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Semesters\FYP\Backend\TheExportersLoom-Apis\data\AI Model Data\Shirts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Semesters\FYP\Backend\TheExportersLoom-Apis\data\Shirts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -920,12 +920,12 @@
   <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="36.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>

</xml_diff>